<commit_message>
set hidden value on the components
</commit_message>
<xml_diff>
--- a/export_logsheet.xlsx
+++ b/export_logsheet.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fas2020\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="7365"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet1'!$A$1:$O$31</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>OFFICE</t>
   </si>
@@ -35,9 +30,15 @@
     <t>QUALITY PROCEDURE TITLE</t>
   </si>
   <si>
+    <t>Website Administration</t>
+  </si>
+  <si>
     <t>QUALITY OBJECTIVE</t>
   </si>
   <si>
+    <t>2. 85% Timely posting of  information on the website within three (3) hours upon receipt of request or within agreed timeline.</t>
+  </si>
+  <si>
     <t>FREQUENCY OF MONITORING:</t>
   </si>
   <si>
@@ -47,7 +48,19 @@
     <t xml:space="preserve">PERIOD: </t>
   </si>
   <si>
+    <t xml:space="preserve">Month of </t>
+  </si>
+  <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of posted information on the website within three (3) hours upon receipt of request or within agreed timeline </t>
+  </si>
+  <si>
+    <t>Total number of request for posting of information on the website</t>
+  </si>
+  <si>
+    <t>Objective 2 Results</t>
   </si>
   <si>
     <t>Notes</t>
@@ -61,24 +74,27 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <u/>
+        <rFont val="Cambria"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
         <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
+        <u val="single"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <rFont val="Cambria"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
         <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
+        <u val="none"/>
       </rPr>
-      <t>&gt;                           85%</t>
+      <t xml:space="preserve">&gt;                           85%</t>
     </r>
   </si>
   <si>
@@ -87,114 +103,103 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <u/>
+        <rFont val="Cambria"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
         <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
+        <u val="single"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <rFont val="Cambria"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FF000000"/>
         <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
+        <u val="none"/>
       </rPr>
-      <t>&gt;                           85%</t>
+      <t xml:space="preserve">&gt;                           85%</t>
     </r>
   </si>
   <si>
     <t>Remarks (Indicate reason if target is unmet)</t>
-  </si>
-  <si>
-    <t>Website Administration</t>
-  </si>
-  <si>
-    <t>2. 85% Timely posting of  information on the website within three (3) hours upon receipt of request or within agreed timeline.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Month of </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of posted information on the website within three (3) hours upon receipt of request or within agreed timeline </t>
-  </si>
-  <si>
-    <t>Total number of request for posting of information on the website</t>
-  </si>
-  <si>
-    <t>Objective 2 Results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -211,20 +216,13 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="26">
+  <borders count="13">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -239,450 +237,254 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="53">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="9" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -698,7 +500,7 @@
     <xdr:ext cx="1247775" cy="1200150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 4"/>
+        <xdr:cNvPr id="1" name="Picture 4" descr=""/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -710,10 +512,7 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
+        <a:xfrm rot="0"/>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -721,94 +520,66 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>127350</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>151916</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>183809</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>50759</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="2933700" cy="847725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 2" descr=""/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1378024" y="151916"/>
-          <a:ext cx="2930524" cy="851343"/>
-        </a:xfrm>
+        <a:xfrm rot="0"/>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2073</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>173936</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>330350</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>30501</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="3076575" cy="809625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="3" name="Picture 4" descr=""/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7850673" y="173936"/>
-          <a:ext cx="3081002" cy="809065"/>
-        </a:xfrm>
+        <a:xfrm rot="0"/>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -855,7 +626,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -890,7 +661,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1098,31 +869,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A9:O47"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:O13"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="55" view="pageLayout" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="true" style="0"/>
+    <col min="2" max="2" width="24.7109375" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.7109375" hidden="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="8.85546875" hidden="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="15.28515625" customWidth="true" style="0"/>
+    <col min="8" max="8" width="11.28515625" customWidth="true" style="0"/>
+    <col min="9" max="9" width="10.85546875" customWidth="true" style="0"/>
+    <col min="10" max="10" width="11.28515625" customWidth="true" style="0"/>
+    <col min="11" max="11" width="11.42578125" customWidth="true" style="0"/>
+    <col min="15" max="15" width="5.5703125" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="K1"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="23" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +920,7 @@
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="36" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +928,7 @@
       <c r="C10" s="37"/>
       <c r="D10" s="38"/>
       <c r="E10" s="19" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -1164,15 +941,15 @@
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="27"/>
       <c r="E11" s="16" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -1185,15 +962,15 @@
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -1206,15 +983,15 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" s="52"/>
       <c r="C13" s="52"/>
       <c r="D13" s="52"/>
       <c r="E13" s="21" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
@@ -1227,7 +1004,7 @@
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1244,21 +1021,21 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" customHeight="1" ht="14.45">
       <c r="A15" s="35" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
       <c r="E15" s="30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="45" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H15" s="46"/>
       <c r="I15" s="46"/>
@@ -1266,12 +1043,12 @@
       <c r="K15" s="47"/>
       <c r="L15" s="48"/>
       <c r="M15" s="39" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="N15" s="40"/>
       <c r="O15" s="41"/>
     </row>
-    <row r="16" spans="1:15" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" customHeight="1" ht="67.15">
       <c r="A16" s="35"/>
       <c r="B16" s="34"/>
       <c r="C16" s="6"/>
@@ -1279,16 +1056,16 @@
       <c r="E16" s="32"/>
       <c r="F16" s="33"/>
       <c r="G16" s="10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J16" s="49" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="K16" s="50"/>
       <c r="L16" s="51"/>
@@ -1296,7 +1073,7 @@
       <c r="N16" s="43"/>
       <c r="O16" s="44"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1313,7 +1090,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1330,7 +1107,7 @@
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1347,7 +1124,7 @@
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1364,7 +1141,7 @@
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1381,7 +1158,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1398,7 +1175,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1415,7 +1192,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1432,7 +1209,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1449,7 +1226,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1466,7 +1243,7 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1483,7 +1260,7 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1500,7 +1277,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1517,7 +1294,7 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1534,7 +1311,7 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1551,7 +1328,7 @@
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1568,7 +1345,7 @@
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1585,7 +1362,7 @@
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1602,7 +1379,7 @@
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1619,7 +1396,7 @@
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1636,7 +1413,7 @@
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1653,7 +1430,7 @@
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1670,7 +1447,7 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1687,7 +1464,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1704,7 +1481,7 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1721,7 +1498,7 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1738,7 +1515,7 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1755,7 +1532,7 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1772,7 +1549,7 @@
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1789,7 +1566,7 @@
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1806,7 +1583,7 @@
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1824,8 +1601,8 @@
       <c r="O47" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="30">
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="C15:D15"/>
@@ -1857,44 +1634,80 @@
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
   </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.25" right="0.25" top="0.2" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;C&amp;"+,Regular"&amp;10&amp;K00-024THIS DOCUMENTED INFORMATION IS CONTROLLED AND NOT TO BE REPRODUCED WITHOUT AUTHORIZATION&amp;"Calibri,Regular"&amp;11&amp;K000000
+  <pageSetup paperSize="9" orientation="landscape" scale="92" fitToHeight="0" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"+,Regular"&amp;10&amp;K00-024THIS DOCUMENTED INFORMATION IS CONTROLLED AND NOT TO BE REPRODUCED WITHOUT AUTHORIZATION&amp;"Calibri,Regular"&amp;11&amp;K000000
 </oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="47" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="15" max="1048575" man="1"/>
+    <brk id="15" man="1"/>
   </colBreaks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>